<commit_message>
extract by zuh eid
</commit_message>
<xml_diff>
--- a/csv/xls/travelsky_09053_except.xlsx
+++ b/csv/xls/travelsky_09053_except.xlsx
@@ -441,7 +441,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>business_class</t>
+          <t>business_short</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -466,7 +466,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>登录按钮</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -491,7 +491,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>旅客检索页面加载</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -516,7 +516,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>用户注销按钮</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -541,7 +541,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>登录按钮</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -566,7 +566,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>旅客检索页面加载</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -591,7 +591,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>用户临时退出页面加载</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -616,7 +616,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>登录按钮</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -641,7 +641,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>旅客检索页面加载</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -666,7 +666,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>用户注销按钮</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -691,7 +691,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>登录按钮</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -716,7 +716,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>旅客检索页面加载</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -741,7 +741,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>旅客检索清空按钮</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -766,7 +766,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>旅客检索清空按钮</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -791,7 +791,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>登录按钮</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -816,7 +816,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>旅客检索页面加载</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -841,7 +841,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>用户注销按钮</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -866,7 +866,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>登录按钮</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -891,7 +891,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>旅客检索页面加载</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -916,7 +916,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>用户注销按钮</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -941,7 +941,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>登录按钮</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -966,7 +966,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>旅客检索页面加载</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -991,7 +991,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>用户注销按钮</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1016,7 +1016,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>登录按钮</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1041,7 +1041,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>旅客检索页面加载</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1066,7 +1066,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>用户注销按钮</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1091,7 +1091,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>登录按钮</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1241,7 +1241,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>用户注销按钮</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1266,7 +1266,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>登录按钮</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1291,7 +1291,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>旅客检索页面加载</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1316,7 +1316,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>用户注销按钮</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1341,7 +1341,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>登录按钮</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1366,7 +1366,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>旅客检索页面加载</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1391,7 +1391,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>用户注销按钮</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1416,7 +1416,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>用户注销按钮</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1441,7 +1441,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>登录按钮</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1466,7 +1466,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>旅客检索页面加载</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1491,7 +1491,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>用户注销按钮</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1516,7 +1516,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>用户注销按钮</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1541,7 +1541,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>登录按钮</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1566,7 +1566,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>旅客检索页面加载</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1591,7 +1591,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>用户注销按钮</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1616,7 +1616,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>登录按钮</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1641,7 +1641,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>旅客检索页面加载</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1666,7 +1666,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>登录按钮</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -1691,7 +1691,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>旅客检索页面加载</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -1716,7 +1716,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>用户注销按钮</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -1741,7 +1741,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>登录按钮</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -1766,7 +1766,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>登录按钮</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -1816,7 +1816,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>旅客检索页面加载</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -1841,7 +1841,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>登录按钮</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -1866,7 +1866,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>旅客检索页面加载</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -1891,7 +1891,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>用户注销按钮</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -1916,7 +1916,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>登录按钮</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -1966,7 +1966,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>用户注销按钮</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -1991,7 +1991,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>登录按钮</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -2016,7 +2016,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>旅客检索页面加载</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -2041,7 +2041,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>用户注销按钮</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -2066,7 +2066,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>登录按钮</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -2166,7 +2166,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>旅客详情刷新按钮</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -2176,7 +2176,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>旅客详情</t>
         </is>
       </c>
     </row>
@@ -2191,7 +2191,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>旅客详情刷新按钮</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -2201,7 +2201,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>旅客详情</t>
         </is>
       </c>
     </row>
@@ -2291,7 +2291,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>列表切换旅客</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -2316,7 +2316,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>旅客详情刷新按钮</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -2326,7 +2326,7 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>旅客详情</t>
         </is>
       </c>
     </row>
@@ -2341,7 +2341,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>旅客详情刷新按钮</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -2351,7 +2351,7 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>旅客详情</t>
         </is>
       </c>
     </row>
@@ -2366,7 +2366,7 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>旅客详情刷新按钮</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -2376,7 +2376,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>旅客详情</t>
         </is>
       </c>
     </row>
@@ -2391,7 +2391,7 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>旅客详情刷新按钮</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -2401,7 +2401,7 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>旅客详情</t>
         </is>
       </c>
     </row>
@@ -2416,7 +2416,7 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>旅客详情刷新按钮</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -2426,7 +2426,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>旅客详情</t>
         </is>
       </c>
     </row>
@@ -2441,7 +2441,7 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>旅客详情刷新按钮</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -2451,7 +2451,7 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>旅客详情</t>
         </is>
       </c>
     </row>
@@ -2466,7 +2466,7 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>旅客详情刷新按钮</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -2476,7 +2476,7 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>旅客详情</t>
         </is>
       </c>
     </row>
@@ -2491,7 +2491,7 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>旅客详情刷新按钮</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -2501,7 +2501,7 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>旅客详情</t>
         </is>
       </c>
     </row>
@@ -2516,7 +2516,7 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>列表切换旅客</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -2541,7 +2541,7 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>旅客详情刷新按钮</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -2551,7 +2551,7 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>旅客详情</t>
         </is>
       </c>
     </row>
@@ -2566,7 +2566,7 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>旅客详情刷新按钮</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -2576,7 +2576,7 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>旅客详情</t>
         </is>
       </c>
     </row>
@@ -2591,7 +2591,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>旅客详情刷新按钮</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -2601,7 +2601,7 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>旅客详情</t>
         </is>
       </c>
     </row>
@@ -2641,7 +2641,7 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>旅客详情刷新按钮</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -2651,7 +2651,7 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>旅客详情</t>
         </is>
       </c>
     </row>
@@ -2666,7 +2666,7 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>旅客详情刷新按钮</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -2676,7 +2676,7 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>旅客详情</t>
         </is>
       </c>
     </row>
@@ -2691,7 +2691,7 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>旅客详情刷新按钮</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -2701,7 +2701,7 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>旅客详情</t>
         </is>
       </c>
     </row>
@@ -2716,7 +2716,7 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>旅客详情刷新按钮</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
@@ -2726,7 +2726,7 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>旅客详情</t>
         </is>
       </c>
     </row>
@@ -2741,7 +2741,7 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>旅客检索页面加载</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -2766,7 +2766,7 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>用户注销按钮</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
@@ -2791,7 +2791,7 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>登录按钮</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -2841,7 +2841,7 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>用户注销按钮</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -2866,7 +2866,7 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>登录按钮</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
@@ -2891,7 +2891,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>旅客检索页面加载</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -2916,7 +2916,7 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>用户注销按钮</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -2941,7 +2941,7 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>登录按钮</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -2966,7 +2966,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>旅客检索页面加载</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -2991,7 +2991,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>38</t>
+          <t>已登机查询按钮</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -3001,7 +3001,7 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>已/未登机查询</t>
+          <t>已/未登机查询入口</t>
         </is>
       </c>
     </row>
@@ -3016,7 +3016,7 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>登录按钮</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -3041,7 +3041,7 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>旅客检索页面加载</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -3066,7 +3066,7 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>旅客提取页签检索按钮</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -3091,7 +3091,7 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>重打登机牌按钮</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -3101,7 +3101,7 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>重打牌</t>
+          <t>重打牌登机牌</t>
         </is>
       </c>
     </row>
@@ -3116,7 +3116,7 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>重打登机牌按钮</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -3126,7 +3126,7 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>重打牌</t>
+          <t>重打牌登机牌</t>
         </is>
       </c>
     </row>
@@ -3141,7 +3141,7 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>旅客提取页签检索按钮</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -3166,7 +3166,7 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>序号输入框选中旅客</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -3191,7 +3191,7 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>重打登机牌按钮</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
@@ -3201,7 +3201,7 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>重打牌</t>
+          <t>重打牌登机牌</t>
         </is>
       </c>
     </row>
@@ -3216,7 +3216,7 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>重打登机牌按钮</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -3226,7 +3226,7 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>重打牌</t>
+          <t>重打牌登机牌</t>
         </is>
       </c>
     </row>
@@ -3241,7 +3241,7 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>旅客提取页签检索按钮</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
@@ -3266,7 +3266,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>序号输入框选中旅客</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -3291,7 +3291,7 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>重打登机牌按钮</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
@@ -3301,7 +3301,7 @@
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>重打牌</t>
+          <t>重打牌登机牌</t>
         </is>
       </c>
     </row>
@@ -3316,7 +3316,7 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>重打登机牌按钮</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
@@ -3326,7 +3326,7 @@
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>重打牌</t>
+          <t>重打牌登机牌</t>
         </is>
       </c>
     </row>

</xml_diff>